<commit_message>
implemntação do bot de telegram
</commit_message>
<xml_diff>
--- a/datebase/perfis.xlsx
+++ b/datebase/perfis.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="7">
   <si>
     <t xml:space="preserve">Perfis</t>
   </si>
@@ -28,13 +28,19 @@
     <t xml:space="preserve">Enviados</t>
   </si>
   <si>
-    <t xml:space="preserve">Weiwei1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ca1o.henr1que</t>
-  </si>
-  <si>
-    <t xml:space="preserve">davdsantos45</t>
+    <t xml:space="preserve">ca1o_henr1que</t>
+  </si>
+  <si>
+    <t xml:space="preserve">davdsantos45 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">weiwei1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eliana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matue30</t>
   </si>
 </sst>
 </file>
@@ -150,15 +156,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -166,7 +176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
@@ -174,7 +184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
@@ -182,7 +192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
@@ -190,131 +200,99 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="B9" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B12" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="B13" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>2</v>
-      </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>